<commit_message>
add search param for researchstudy (todo - add type, target, expression.) update IG footer to remove some HL7 specific stuff. Add extension to cr-core-results profile for researchstudy.
</commit_message>
<xml_diff>
--- a/docs/cr-core-patient.xlsx
+++ b/docs/cr-core-patient.xlsx
@@ -178,7 +178,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">id {[]} {[]}
+    <t xml:space="preserve">id
 </t>
   </si>
   <si>
@@ -197,7 +197,7 @@
     <t>Patient.meta</t>
   </si>
   <si>
-    <t xml:space="preserve">Meta {[]} {[]}
+    <t xml:space="preserve">Meta
 </t>
   </si>
   <si>
@@ -213,7 +213,7 @@
     <t>Patient.implicitRules</t>
   </si>
   <si>
-    <t xml:space="preserve">uri {[]} {[]}
+    <t xml:space="preserve">uri
 </t>
   </si>
   <si>
@@ -232,7 +232,7 @@
     <t>Patient.language</t>
   </si>
   <si>
-    <t xml:space="preserve">code {[]} {[]}
+    <t xml:space="preserve">code
 </t>
   </si>
   <si>
@@ -264,7 +264,7 @@
 htmlxhtmldisplay</t>
   </si>
   <si>
-    <t xml:space="preserve">Narrative {[]} {[]}
+    <t xml:space="preserve">Narrative
 </t>
   </si>
   <si>
@@ -290,7 +290,7 @@
 anonymous resourcescontained resources</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource {[]} {[]}
+    <t xml:space="preserve">Resource
 </t>
   </si>
   <si>
@@ -316,7 +316,7 @@
 user content</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[]} {[]}
+    <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
@@ -342,7 +342,7 @@
 Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
   </si>
   <si>
-    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](extensibility.html#modifierExtension).</t>
+    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://build.fhir.org/extensibility.html#modifierExtension).</t>
   </si>
   <si>
     <t>DomainResource.modifierExtension</t>
@@ -351,7 +351,7 @@
     <t>Patient.identifier</t>
   </si>
   <si>
-    <t xml:space="preserve">Identifier {[]} {[]}
+    <t xml:space="preserve">Identifier
 </t>
   </si>
   <si>
@@ -379,7 +379,7 @@
     <t>Patient.identifier.id</t>
   </si>
   <si>
-    <t xml:space="preserve">string {[]} {[]}
+    <t xml:space="preserve">string
 </t>
   </si>
   <si>
@@ -447,7 +447,7 @@
     <t>Patient.identifier.type</t>
   </si>
   <si>
-    <t xml:space="preserve">CodeableConcept {[]} {[]}
+    <t xml:space="preserve">CodeableConcept
 </t>
   </si>
   <si>
@@ -493,7 +493,7 @@
     <t>There are many sets  of identifiers.  To perform matching of two identifiers, we need to know what set we're dealing with. The system identifies a particular set of unique identifiers.</t>
   </si>
   <si>
-    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://www.acme.com/identifiers/patient"/&gt;</t>
+    <t>http://www.acme.com/identifiers/patient</t>
   </si>
   <si>
     <t>Identifier.system</t>
@@ -514,10 +514,10 @@
     <t>The portion of the identifier typically relevant to the user and which is unique within the context of the system.</t>
   </si>
   <si>
-    <t>If the value is a full URI, then the system SHALL be urn:ietf:rfc:3986.  The value's primary purpose is computational mapping.  As a result, it may be normalized for comparison purposes (e.g. removing non-significant whitespace, dashes, etc.)  A value formatted for human display can be conveyed using the [Rendered Value extension](extension-rendered-value.html). Identifier.value is to be treated as case sensitive unless knowledge of the Identifier.system allows the processer to be confident that non-case-sensitive processing is safe.</t>
-  </si>
-  <si>
-    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="123456"/&gt;</t>
+    <t>If the value is a full URI, then the system SHALL be urn:ietf:rfc:3986.  The value's primary purpose is computational mapping.  As a result, it may be normalized for comparison purposes (e.g. removing non-significant whitespace, dashes, etc.)  A value formatted for human display can be conveyed using the [Rendered Value extension](http://build.fhir.org/extension-rendered-value.html). Identifier.value is to be treated as case sensitive unless knowledge of the Identifier.system allows the processer to be confident that non-case-sensitive processing is safe.</t>
+  </si>
+  <si>
+    <t>123456</t>
   </si>
   <si>
     <t>Identifier.value</t>
@@ -532,7 +532,7 @@
     <t>Patient.identifier.period</t>
   </si>
   <si>
-    <t xml:space="preserve">Period {[]} {[]}
+    <t xml:space="preserve">Period
 </t>
   </si>
   <si>
@@ -554,7 +554,7 @@
     <t>Patient.identifier.assigner</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Organization]]}
+    <t xml:space="preserve">Reference(Organization)
 </t>
   </si>
   <si>
@@ -579,7 +579,7 @@
     <t>Patient.active</t>
   </si>
   <si>
-    <t xml:space="preserve">boolean {[]} {[]}
+    <t xml:space="preserve">boolean
 </t>
   </si>
   <si>
@@ -610,7 +610,7 @@
     <t>Patient.name</t>
   </si>
   <si>
-    <t xml:space="preserve">HumanName {[]} {[]}
+    <t xml:space="preserve">HumanName
 </t>
   </si>
   <si>
@@ -638,7 +638,7 @@
     <t>Patient.telecom</t>
   </si>
   <si>
-    <t xml:space="preserve">ContactPoint {[]} {[]}
+    <t xml:space="preserve">ContactPoint
 </t>
   </si>
   <si>
@@ -696,7 +696,7 @@
     <t>Patient.birthDate</t>
   </si>
   <si>
-    <t xml:space="preserve">date {[]} {[]}
+    <t xml:space="preserve">date
 </t>
   </si>
   <si>
@@ -727,8 +727,8 @@
     <t>Patient.deceased[x]</t>
   </si>
   <si>
-    <t>boolean {[]} {[]}
-dateTime {[]} {[]}</t>
+    <t>boolean
+dateTime</t>
   </si>
   <si>
     <t>Indicates if the individual is deceased or not</t>
@@ -752,7 +752,7 @@
     <t>Patient.address</t>
   </si>
   <si>
-    <t xml:space="preserve">Address {[]} {[]}
+    <t xml:space="preserve">Address
 </t>
   </si>
   <si>
@@ -807,8 +807,8 @@
     <t>Patient.multipleBirth[x]</t>
   </si>
   <si>
-    <t>boolean {[]} {[]}
-integer {[]} {[]}</t>
+    <t>boolean
+integer</t>
   </si>
   <si>
     <t>Whether patient is part of a multiple birth</t>
@@ -832,7 +832,7 @@
     <t>Patient.photo</t>
   </si>
   <si>
-    <t xml:space="preserve">Attachment {[]} {[]}
+    <t xml:space="preserve">Attachment
 </t>
   </si>
   <si>
@@ -860,7 +860,7 @@
     <t>Patient.contact</t>
   </si>
   <si>
-    <t xml:space="preserve">BackboneElement {[]} {[]}
+    <t xml:space="preserve">BackboneElement
 </t>
   </si>
   <si>
@@ -1110,7 +1110,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Organization], CanonicalType[http://hl7.org/fhir/StructureDefinition/Practitioner], CanonicalType[http://hl7.org/fhir/StructureDefinition/PractitionerRole]]}
+    <t xml:space="preserve">Reference(Organization|Practitioner|PractitionerRole)
 </t>
   </si>
   <si>
@@ -1181,7 +1181,7 @@
     <t>Patient.link.other</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Patient], CanonicalType[http://hl7.org/fhir/StructureDefinition/RelatedPerson]]}
+    <t xml:space="preserve">Reference(Patient|RelatedPerson)
 </t>
   </si>
   <si>
@@ -1262,67 +1262,67 @@
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin"/>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin"/>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin"/>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
   </borders>
@@ -1358,7 +1358,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO54"/>
+  <dimension ref="A1:AN54"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>

</xml_diff>